<commit_message>
copy changes to template and other barangays
</commit_message>
<xml_diff>
--- a/barangay/admin/reports/excel/template.xlsx
+++ b/barangay/admin/reports/excel/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\indang.gov.ph\do-not-delete-this\admin\reports\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2290CDC1-A221-4F8E-ACFA-7F8A400CFBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1DB1D5-5141-4439-8FB3-51696AB8C4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="9975" yWindow="3615" windowWidth="12315" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL-Resident-report" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -568,10 +568,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -583,6 +579,13 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -942,12 +945,12 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
@@ -962,143 +965,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="10"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="10"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
revisions PO and reports
</commit_message>
<xml_diff>
--- a/barangay/admin/reports/excel/template.xlsx
+++ b/barangay/admin/reports/excel/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\indang.gov.ph\barangay\admin\reports\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EB7343-5DC6-4332-8DFD-D4C24AF6D50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48566AC7-16C6-4764-8ADF-1113A953FFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Marital</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Religion</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>Date record</t>
+  </si>
+  <si>
+    <t>Sex</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,22 +565,22 @@
         <v>6</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update PO and reports by mads
</commit_message>
<xml_diff>
--- a/barangay/admin/reports/excel/template.xlsx
+++ b/barangay/admin/reports/excel/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\indang.gov.ph\barangay\admin\reports\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48566AC7-16C6-4764-8ADF-1113A953FFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16F4A58-FB68-4E92-94D1-FF30B4510D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,45 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>Firstname</t>
-  </si>
-  <si>
-    <t>Middle</t>
-  </si>
-  <si>
-    <t>Suffix</t>
-  </si>
-  <si>
-    <t>Birthdate</t>
-  </si>
-  <si>
-    <t>Marital</t>
-  </si>
-  <si>
-    <t>Religion</t>
-  </si>
-  <si>
-    <t>Nationality</t>
-  </si>
-  <si>
-    <t>Occupation</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Date record</t>
-  </si>
-  <si>
-    <t>Sex</t>
   </si>
 </sst>
 </file>
@@ -81,7 +45,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -109,7 +72,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -117,11 +80,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,7 +430,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +448,7 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -497,7 +463,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -512,7 +478,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -527,7 +493,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -542,46 +508,23 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -591,5 +534,6 @@
     <mergeCell ref="A3:M3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>